<commit_message>
Added more stats to ResultsTracker
</commit_message>
<xml_diff>
--- a/src/main/resources/result-tracker.xlsx
+++ b/src/main/resources/result-tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/achan625_uwo_ca/Documents/Coding/BlackjackSimulator/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{0AF35517-C79C-4059-AFB4-5399EA0E15D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EC221CE-6E52-49E2-91C6-D350BE31CC17}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="8_{0AF35517-C79C-4059-AFB4-5399EA0E15D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB9C7865-DC88-4B82-B0C4-18687EA2BECF}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="840" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Round</t>
   </si>
@@ -81,16 +81,26 @@
   </si>
   <si>
     <t>Net Loss</t>
+  </si>
+  <si>
+    <t>Win %</t>
+  </si>
+  <si>
+    <t>Push %</t>
+  </si>
+  <si>
+    <t>Loss %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -130,11 +140,13 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -455,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -464,7 +476,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
@@ -474,17 +486,17 @@
     <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>10</v>
       </c>
@@ -528,7 +540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L3" t="s">
         <v>13</v>
       </c>
@@ -537,7 +549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
         <v>14</v>
       </c>
@@ -546,7 +558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>15</v>
       </c>
@@ -555,12 +567,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L6" t="s">
         <v>11</v>
       </c>
       <c r="M6" s="3" t="e">
         <f>M5/M2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L8" t="str">
+        <f>_xlfn.CONCAT(C1, " %")</f>
+        <v>BLACKJACK %</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ref="M8:S8" si="0">_xlfn.CONCAT(D1, " %")</f>
+        <v>WIN %</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_WIN %</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>PUSH %</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_BUST %</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v>BUST %</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_LOSE %</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>LOSE %</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L9" s="5" t="e">
+        <f>SUM(C:C)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="5" t="e">
+        <f t="shared" ref="M9:S9" si="1">SUM(D:D)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="4" t="e">
+        <f>SUM(C:E)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="4" t="e">
+        <f>SUM(F:F)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="4" t="e">
+        <f>SUM(G:J)/SUM(C:J)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>